<commit_message>
Update analysis results and charts
- Updated all chart visualizations in charts/ folder
- Updated analysis results in outputs/ folder
- Updated Excel files with latest group metrics
- Updated CSV files with latest performance metrics
- All Python analysis scripts included
- Excluded presentation summary as requested
</commit_message>
<xml_diff>
--- a/health-bias-audit/outputs/group_metrics_base.xlsx
+++ b/health-bias-audit/outputs/group_metrics_base.xlsx
@@ -481,85 +481,85 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Man</t>
+          <t>Non-binary</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2417582417582418</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.04019664545980337</v>
+        <v>-0.5413533834586466</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9166666666666666</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.02083333333333337</v>
+        <v>-0.9927536231884058</v>
       </c>
       <c r="G2" t="n">
-        <v>0.02108699680485284</v>
+        <v>2.377935733887305e-10</v>
       </c>
       <c r="H2" t="n">
-        <v>0.001154092218706278</v>
+        <v>-0.02671138269588797</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Woman</t>
+          <t>Man</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2988505747126437</v>
+        <v>0.4473684210526316</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01689568749459858</v>
+        <v>-0.093984962406015</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9454545454545454</v>
+        <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.007954545454545436</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01944388443948288</v>
+        <v>0.03308232690219727</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0004890201466636844</v>
+        <v>0.006370943968515726</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Non-binary</t>
+          <t>Woman</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>189</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0.582010582010582</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7180451127819549</v>
+        <v>0.04065719855193539</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>0.9905660377358491</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0625</v>
+        <v>-0.002187585452556706</v>
       </c>
       <c r="G4" t="n">
-        <v>1.820335594311874e-08</v>
+        <v>0.02429085193415082</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.01993288638279062</v>
+        <v>-0.002420530999530723</v>
       </c>
     </row>
   </sheetData>
@@ -573,7 +573,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,7 +626,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dutch</t>
+          <t>Croatian</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -636,355 +636,299 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.5413533834586466</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.9375</v>
+        <v>-0.9927536231884058</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004509563310678995</v>
+        <v>0.0006130258047512081</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.01542334127546757</v>
+        <v>-0.02609835712893033</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Japanese</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.1663533834586466</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.9375</v>
+        <v>-0.2427536231884058</v>
       </c>
       <c r="G3" t="n">
-        <v>1.519564302464107e-08</v>
+        <v>0.04952669376063773</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.01993288939050354</v>
+        <v>0.02281531082695619</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Portuguese</t>
+          <t>English</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.1413533834586466</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.9375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G4" t="n">
-        <v>0.05140149336806196</v>
+        <v>0.007208463115822105</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0314685887819154</v>
+        <v>-0.01950291981785944</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Romanian</t>
+          <t>Italian</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.04135338345864659</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.9375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G5" t="n">
-        <v>0.009624592024271694</v>
+        <v>0.01091044529753344</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.01030831256187487</v>
+        <v>-0.0158009376361481</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Russian</t>
+          <t>Romanian</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.04135338345864659</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G6" t="n">
-        <v>0.001236819638662418</v>
+        <v>0.0002163129610653677</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.01869608494748415</v>
+        <v>-0.02649506997261617</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Spanish</t>
+          <t>French</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>0.5283018867924528</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.2819548872180451</v>
+        <v>-0.01305149666619376</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.9375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G7" t="n">
-        <v>1.974365758494905e-06</v>
+        <v>0.02901499345507749</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.01993093022038807</v>
+        <v>0.002303610521395948</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vietnamese</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.2819548872180451</v>
+        <v>0.2086466165413534</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.9375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G8" t="n">
-        <v>0.001060189120945766</v>
+        <v>0.02575229467046115</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.0188727154652008</v>
+        <v>-0.0009590882632203937</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Italian</t>
+          <t>Arab</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.09090909090909091</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.1910457963089542</v>
+        <v>0.4586466165413534</v>
       </c>
       <c r="E9" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.4375</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G9" t="n">
-        <v>0.02545880096512923</v>
+        <v>2.183694983766856e-05</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00552589637898266</v>
+        <v>-0.02668954598384388</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Portuguese</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.03195488721804512</v>
+        <v>0.4586466165413534</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G10" t="n">
-        <v>0.009783040508978606</v>
+        <v>0.02203319115004268</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.01014986407716796</v>
+        <v>-0.00467819178363886</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Russian</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2727272727272727</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.009227614490772418</v>
+        <v>0.4586466165413534</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G11" t="n">
-        <v>0.008093868358683712</v>
+        <v>0.008786489787561962</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.01183903622746285</v>
+        <v>-0.01792489314611958</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>French</t>
+          <t>Turkish</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>216</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2962962962962963</v>
+        <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01434140907825115</v>
+        <v>0.4586466165413534</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>0.003676470588235281</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01964985629815744</v>
+        <v>2.274326564742327e-07</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0002830482879891301</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>German</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.4166666666666667</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.1347117794486216</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.0625</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.03552465676353439</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.01559175217738782</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0.7180451127819549</v>
-      </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.0625</v>
-      </c>
-      <c r="G14" t="n">
-        <v>3.069858399400037e-07</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-0.01993259760030663</v>
+        <v>-0.02671115550102507</v>
       </c>
     </row>
   </sheetData>
@@ -1051,57 +995,57 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Non-German</t>
+          <t>German</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>254</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2755905511811024</v>
+        <v>0.375</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.006364336036942753</v>
+        <v>-0.1663533834586466</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.75</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.004166666666666652</v>
+        <v>-0.2427536231884058</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01919628637304163</v>
+        <v>0.04952669376063773</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.0007366182131049344</v>
+        <v>0.02281531082695619</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>German</t>
+          <t>Non-German</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.5465116279069767</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1347117794486216</v>
+        <v>0.005158244448330129</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03552465676353439</v>
+        <v>0.02600393143517128</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01559175217738782</v>
+        <v>-0.0007074514985102656</v>
       </c>
     </row>
   </sheetData>
@@ -1168,141 +1112,141 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mmed2</t>
+          <t>Mmed3</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08823529411764706</v>
+        <v>0.2413793103448276</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.193719593100398</v>
+        <v>-0.299974073113819</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G2" t="n">
-        <v>0.008145703689710427</v>
+        <v>0.009841289206476313</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.01178720089643614</v>
+        <v>-0.01687009372720523</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mmed3</t>
+          <t>Mmed1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1481481481481481</v>
+        <v>0.45</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.133806739069897</v>
+        <v>-0.09135338345864658</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G3" t="n">
-        <v>0.006939947078102714</v>
+        <v>0.01272748592356357</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.01299295750804385</v>
+        <v>-0.01398389701011797</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bmed1</t>
+          <t>Mmed2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2941176470588235</v>
+        <v>0.45</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01216275984077841</v>
+        <v>-0.09135338345864658</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.02840909090909094</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01691664749674199</v>
+        <v>0.02181056550004147</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.003016257089404572</v>
+        <v>-0.004900817433640074</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mmed1</t>
+          <t>Bmed3</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3055555555555556</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02360066833751046</v>
+        <v>0.03007518796992481</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0625</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01634106549443995</v>
+        <v>0.03513777886965821</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.003591839091706614</v>
+        <v>0.008426395935976671</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bmed3</t>
+          <t>Bmed1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C6" t="n">
-        <v>0.34</v>
+        <v>0.6268656716417911</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0580451127819549</v>
+        <v>0.08551228818314449</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.975609756097561</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00694444444444442</v>
+        <v>-0.01714386709084481</v>
       </c>
       <c r="G6" t="n">
-        <v>0.02919430589252257</v>
+        <v>0.03254799485066859</v>
       </c>
       <c r="H6" t="n">
-        <v>0.009261401306376007</v>
+        <v>0.005836611916987051</v>
       </c>
     </row>
     <row r="7">
@@ -1312,25 +1256,25 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C7" t="n">
-        <v>0.392156862745098</v>
+        <v>0.7560975609756098</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1102019755270529</v>
+        <v>0.2147441775169632</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.02840909090909094</v>
+        <v>0.007246376811594235</v>
       </c>
       <c r="G7" t="n">
-        <v>0.03214694982650267</v>
+        <v>0.03745955114193237</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0122140452403561</v>
+        <v>0.01074816820825083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>